<commit_message>
import mysql.connector as mariadb
</commit_message>
<xml_diff>
--- a/wico/数据表结构.xlsx
+++ b/wico/数据表结构.xlsx
@@ -16,7 +16,7 @@
     <sheet name="客户正式投诉" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'不良类型（上传，下载）'!$B$3:$E$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'不良类型（上传，下载）'!$B$3:$E$106</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'零件清单（下载）'!$B$3:$K$152</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'座椅配置（下载）'!$B$3:$E$677</definedName>
   </definedNames>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3827" uniqueCount="1056">
   <si>
     <t>SLIDE ADJR OUT L,FR SEAT</t>
   </si>
@@ -2414,10 +2414,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>绕性轴（长）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>扇形齿</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3296,10 +3292,6 @@
   </si>
   <si>
     <t>更换端盖</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>电动滑轨</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -3593,7 +3585,55 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>滑动拉力过大</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>手动滑轨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>涂润滑油，反复作动</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>更换滑轨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>电动滑轨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑动晃动</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换滑轨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>轴弯曲了</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>绕性轴（短）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换绕性轴</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>绕性轴（长）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换齿轮箱、短轴</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑轨震动并且晃动</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6440,10 +6480,10 @@
         <v>342</v>
       </c>
       <c r="F4" s="19" t="s">
+        <v>721</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>722</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>723</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>65</v>
@@ -6471,10 +6511,10 @@
         <v>64</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>65</v>
@@ -6502,10 +6542,10 @@
         <v>68</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>65</v>
@@ -6533,10 +6573,10 @@
         <v>71</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>2</v>
@@ -6564,10 +6604,10 @@
         <v>310</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>65</v>
@@ -6595,7 +6635,7 @@
         <v>329</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>330</v>
@@ -6626,7 +6666,7 @@
         <v>329</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>330</v>
@@ -6657,7 +6697,7 @@
         <v>329</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>330</v>
@@ -6688,7 +6728,7 @@
         <v>329</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>330</v>
@@ -6719,10 +6759,10 @@
         <v>355</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>2</v>
@@ -6750,10 +6790,10 @@
         <v>103</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>65</v>
@@ -6781,10 +6821,10 @@
         <v>358</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>65</v>
@@ -6812,7 +6852,7 @@
         <v>417</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>418</v>
@@ -6843,10 +6883,10 @@
         <v>313</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>2</v>
@@ -6874,10 +6914,10 @@
         <v>316</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>2</v>
@@ -6905,7 +6945,7 @@
         <v>320</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>321</v>
@@ -6936,7 +6976,7 @@
         <v>320</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>321</v>
@@ -6967,7 +7007,7 @@
         <v>320</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>321</v>
@@ -6998,7 +7038,7 @@
         <v>320</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>321</v>
@@ -7029,7 +7069,7 @@
         <v>106</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>80</v>
@@ -7060,10 +7100,10 @@
         <v>109</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>65</v>
@@ -7091,10 +7131,10 @@
         <v>112</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>65</v>
@@ -7122,7 +7162,7 @@
         <v>173</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>116</v>
@@ -7134,7 +7174,7 @@
         <v>58109</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K26" s="7">
         <v>0</v>
@@ -7157,7 +7197,7 @@
         <v>173</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>116</v>
@@ -7169,7 +7209,7 @@
         <v>58109</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K27" s="7">
         <v>0</v>
@@ -7192,7 +7232,7 @@
         <v>115</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>116</v>
@@ -7202,7 +7242,7 @@
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K28" s="7">
         <v>0</v>
@@ -7225,7 +7265,7 @@
         <v>178</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>116</v>
@@ -7237,7 +7277,7 @@
         <v>58109</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K29" s="7">
         <v>0</v>
@@ -7260,7 +7300,7 @@
         <v>119</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>116</v>
@@ -7270,7 +7310,7 @@
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K30" s="7">
         <v>0</v>
@@ -7293,7 +7333,7 @@
         <v>262</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>263</v>
@@ -7324,7 +7364,7 @@
         <v>266</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>263</v>
@@ -7355,7 +7395,7 @@
         <v>269</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>270</v>
@@ -7386,7 +7426,7 @@
         <v>262</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>263</v>
@@ -7417,7 +7457,7 @@
         <v>269</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>270</v>
@@ -7448,7 +7488,7 @@
         <v>262</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>263</v>
@@ -7458,7 +7498,7 @@
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="19" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="K36" s="7">
         <v>0</v>
@@ -7481,7 +7521,7 @@
         <v>266</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>263</v>
@@ -7491,7 +7531,7 @@
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="19" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="K37" s="7">
         <v>0</v>
@@ -7508,13 +7548,13 @@
         <v>279</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>280</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>263</v>
@@ -7524,7 +7564,7 @@
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="19" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K38" s="7">
         <v>0</v>
@@ -7541,13 +7581,13 @@
         <v>281</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>282</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>263</v>
@@ -7557,7 +7597,7 @@
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="19" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="K39" s="7">
         <v>0</v>
@@ -7580,7 +7620,7 @@
         <v>296</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>297</v>
@@ -7611,7 +7651,7 @@
         <v>300</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>297</v>
@@ -7642,7 +7682,7 @@
         <v>402</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>297</v>
@@ -7673,7 +7713,7 @@
         <v>402</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>297</v>
@@ -7704,7 +7744,7 @@
         <v>407</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>297</v>
@@ -7735,7 +7775,7 @@
         <v>407</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>297</v>
@@ -7766,7 +7806,7 @@
         <v>143</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>80</v>
@@ -7778,7 +7818,7 @@
         <v>58104</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K46" s="7">
         <v>0</v>
@@ -7801,7 +7841,7 @@
         <v>146</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>80</v>
@@ -7813,7 +7853,7 @@
         <v>58104</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K47" s="7">
         <v>0</v>
@@ -7836,7 +7876,7 @@
         <v>149</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>80</v>
@@ -7848,7 +7888,7 @@
         <v>58104</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K48" s="7">
         <v>0</v>
@@ -7871,7 +7911,7 @@
         <v>152</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>80</v>
@@ -7883,7 +7923,7 @@
         <v>58104</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K49" s="7">
         <v>0</v>
@@ -7906,7 +7946,7 @@
         <v>143</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>80</v>
@@ -7918,7 +7958,7 @@
         <v>58112</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K50" s="7">
         <v>0</v>
@@ -7941,7 +7981,7 @@
         <v>143</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>80</v>
@@ -7950,10 +7990,10 @@
         <v>2</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K51" s="7">
         <v>0</v>
@@ -7976,7 +8016,7 @@
         <v>146</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>80</v>
@@ -7988,7 +8028,7 @@
         <v>58112</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K52" s="7">
         <v>0</v>
@@ -8011,7 +8051,7 @@
         <v>146</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>80</v>
@@ -8020,10 +8060,10 @@
         <v>2</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K53" s="7">
         <v>0</v>
@@ -8046,7 +8086,7 @@
         <v>149</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>80</v>
@@ -8058,7 +8098,7 @@
         <v>58112</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K54" s="7">
         <v>0</v>
@@ -8081,7 +8121,7 @@
         <v>149</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>80</v>
@@ -8090,10 +8130,10 @@
         <v>2</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K55" s="7">
         <v>0</v>
@@ -8116,7 +8156,7 @@
         <v>152</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>80</v>
@@ -8128,7 +8168,7 @@
         <v>58112</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K56" s="7">
         <v>0</v>
@@ -8151,7 +8191,7 @@
         <v>152</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>80</v>
@@ -8160,10 +8200,10 @@
         <v>2</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K57" s="7">
         <v>0</v>
@@ -8183,10 +8223,10 @@
         <v>161</v>
       </c>
       <c r="E58" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="F58" s="19" t="s">
         <v>783</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>784</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>80</v>
@@ -8198,7 +8238,7 @@
         <v>52111</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K58" s="7">
         <v>0</v>
@@ -8221,7 +8261,7 @@
         <v>164</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>80</v>
@@ -8233,7 +8273,7 @@
         <v>52111</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K59" s="7">
         <v>0</v>
@@ -8256,7 +8296,7 @@
         <v>79</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>80</v>
@@ -8266,7 +8306,7 @@
       </c>
       <c r="I60" s="7"/>
       <c r="J60" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K60" s="7">
         <v>0</v>
@@ -8289,7 +8329,7 @@
         <v>83</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>80</v>
@@ -8299,7 +8339,7 @@
       </c>
       <c r="I61" s="7"/>
       <c r="J61" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K61" s="7">
         <v>0</v>
@@ -8322,7 +8362,7 @@
         <v>86</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>80</v>
@@ -8332,7 +8372,7 @@
       </c>
       <c r="I62" s="7"/>
       <c r="J62" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K62" s="7">
         <v>0</v>
@@ -8355,7 +8395,7 @@
         <v>89</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>80</v>
@@ -8365,7 +8405,7 @@
       </c>
       <c r="I63" s="7"/>
       <c r="J63" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K63" s="7">
         <v>0</v>
@@ -8388,7 +8428,7 @@
         <v>167</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>80</v>
@@ -8400,7 +8440,7 @@
         <v>58111</v>
       </c>
       <c r="J64" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K64" s="7">
         <v>0</v>
@@ -8423,7 +8463,7 @@
         <v>170</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>80</v>
@@ -8435,7 +8475,7 @@
         <v>58111</v>
       </c>
       <c r="J65" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K65" s="7">
         <v>0</v>
@@ -8458,7 +8498,7 @@
         <v>92</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>80</v>
@@ -8468,7 +8508,7 @@
       </c>
       <c r="I66" s="7"/>
       <c r="J66" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K66" s="7">
         <v>0</v>
@@ -8491,7 +8531,7 @@
         <v>95</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>80</v>
@@ -8501,7 +8541,7 @@
       </c>
       <c r="I67" s="7"/>
       <c r="J67" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K67" s="7">
         <v>0</v>
@@ -8524,7 +8564,7 @@
         <v>98</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>80</v>
@@ -8534,7 +8574,7 @@
       </c>
       <c r="I68" s="7"/>
       <c r="J68" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K68" s="7">
         <v>0</v>
@@ -8551,13 +8591,13 @@
         <v>99</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>100</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>80</v>
@@ -8567,7 +8607,7 @@
       </c>
       <c r="I69" s="7"/>
       <c r="J69" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K69" s="7">
         <v>0</v>
@@ -8590,7 +8630,7 @@
         <v>421</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>418</v>
@@ -8621,7 +8661,7 @@
         <v>421</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G71" s="7" t="s">
         <v>418</v>
@@ -8652,7 +8692,7 @@
         <v>377</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>378</v>
@@ -8683,7 +8723,7 @@
         <v>256</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G73" s="7" t="s">
         <v>257</v>
@@ -8695,7 +8735,7 @@
         <v>58105</v>
       </c>
       <c r="J73" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K73" s="7">
         <v>0</v>
@@ -8718,10 +8758,10 @@
         <v>373</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H74" s="7" t="s">
         <v>65</v>
@@ -8749,7 +8789,7 @@
         <v>285</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>263</v>
@@ -8780,7 +8820,7 @@
         <v>285</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="G76" s="7" t="s">
         <v>263</v>
@@ -8811,7 +8851,7 @@
         <v>426</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>418</v>
@@ -8842,7 +8882,7 @@
         <v>381</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>382</v>
@@ -8873,7 +8913,7 @@
         <v>381</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>382</v>
@@ -8904,7 +8944,7 @@
         <v>417</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G80" s="7" t="s">
         <v>418</v>
@@ -8935,7 +8975,7 @@
         <v>334</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>257</v>
@@ -8966,7 +9006,7 @@
         <v>334</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G82" s="7" t="s">
         <v>257</v>
@@ -8997,7 +9037,7 @@
         <v>136</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G83" s="7" t="s">
         <v>137</v>
@@ -9007,7 +9047,7 @@
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="19" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="K83" s="7">
         <v>0</v>
@@ -9030,7 +9070,7 @@
         <v>136</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G84" s="7" t="s">
         <v>137</v>
@@ -9040,7 +9080,7 @@
       </c>
       <c r="I84" s="7"/>
       <c r="J84" s="19" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="K84" s="7">
         <v>0</v>
@@ -9063,7 +9103,7 @@
         <v>291</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G85" s="7" t="s">
         <v>292</v>
@@ -9094,7 +9134,7 @@
         <v>413</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G86" s="7" t="s">
         <v>292</v>
@@ -9125,10 +9165,10 @@
         <v>126</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H87" s="7" t="s">
         <v>2</v>
@@ -9156,7 +9196,7 @@
         <v>129</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="G88" s="7" t="s">
         <v>130</v>
@@ -9187,7 +9227,7 @@
         <v>0</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>1</v>
@@ -9199,7 +9239,7 @@
         <v>58108</v>
       </c>
       <c r="J89" s="19" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="K89" s="7">
         <v>0</v>
@@ -9222,7 +9262,7 @@
         <v>7</v>
       </c>
       <c r="F90" s="19" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G90" s="7" t="s">
         <v>1</v>
@@ -9234,7 +9274,7 @@
         <v>58108</v>
       </c>
       <c r="J90" s="19" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="K90" s="7">
         <v>0</v>
@@ -9257,7 +9297,7 @@
         <v>10</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>1</v>
@@ -9269,7 +9309,7 @@
         <v>58108</v>
       </c>
       <c r="J91" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="K91" s="7">
         <v>0</v>
@@ -9292,7 +9332,7 @@
         <v>13</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>1</v>
@@ -9304,7 +9344,7 @@
         <v>58108</v>
       </c>
       <c r="J92" s="19" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="K92" s="7">
         <v>0</v>
@@ -9327,7 +9367,7 @@
         <v>3</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="G93" s="7" t="s">
         <v>1</v>
@@ -9339,7 +9379,7 @@
         <v>58108</v>
       </c>
       <c r="J93" s="19" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="K93" s="7">
         <v>0</v>
@@ -9362,7 +9402,7 @@
         <v>18</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G94" s="7" t="s">
         <v>1</v>
@@ -9374,7 +9414,7 @@
         <v>58108</v>
       </c>
       <c r="J94" s="19" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="K94" s="7">
         <v>0</v>
@@ -9397,7 +9437,7 @@
         <v>21</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>1</v>
@@ -9409,7 +9449,7 @@
         <v>58108</v>
       </c>
       <c r="J95" s="19" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="K95" s="7">
         <v>0</v>
@@ -9432,7 +9472,7 @@
         <v>24</v>
       </c>
       <c r="F96" s="19" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="G96" s="7" t="s">
         <v>1</v>
@@ -9444,7 +9484,7 @@
         <v>58108</v>
       </c>
       <c r="J96" s="19" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="K96" s="7">
         <v>0</v>
@@ -9467,7 +9507,7 @@
         <v>363</v>
       </c>
       <c r="F97" s="19" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>364</v>
@@ -9498,7 +9538,7 @@
         <v>334</v>
       </c>
       <c r="F98" s="19" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>257</v>
@@ -9529,7 +9569,7 @@
         <v>334</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G99" s="7" t="s">
         <v>257</v>
@@ -9560,7 +9600,7 @@
         <v>129</v>
       </c>
       <c r="F100" s="19" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G100" s="7" t="s">
         <v>130</v>
@@ -9591,7 +9631,7 @@
         <v>136</v>
       </c>
       <c r="F101" s="19" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="G101" s="7" t="s">
         <v>137</v>
@@ -9601,7 +9641,7 @@
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="19" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="K101" s="7">
         <v>0</v>
@@ -9618,13 +9658,13 @@
         <v>138</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>139</v>
       </c>
       <c r="F102" s="19" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G102" s="7" t="s">
         <v>137</v>
@@ -9634,7 +9674,7 @@
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="19" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="K102" s="7">
         <v>0</v>
@@ -9657,7 +9697,7 @@
         <v>129</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G103" s="7" t="s">
         <v>130</v>
@@ -9688,7 +9728,7 @@
         <v>74</v>
       </c>
       <c r="F104" s="19" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G104" s="7" t="s">
         <v>75</v>
@@ -9719,7 +9759,7 @@
         <v>122</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G105" s="7" t="s">
         <v>123</v>
@@ -9729,7 +9769,7 @@
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K105" s="7">
         <v>0</v>
@@ -9752,7 +9792,7 @@
         <v>122</v>
       </c>
       <c r="F106" s="19" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G106" s="7" t="s">
         <v>123</v>
@@ -9762,7 +9802,7 @@
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K106" s="7">
         <v>0</v>
@@ -9785,7 +9825,7 @@
         <v>181</v>
       </c>
       <c r="F107" s="19" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G107" s="7" t="s">
         <v>182</v>
@@ -9797,7 +9837,7 @@
         <v>58103</v>
       </c>
       <c r="J107" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K107" s="7">
         <v>0</v>
@@ -9820,7 +9860,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="19" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>182</v>
@@ -9832,7 +9872,7 @@
         <v>58103</v>
       </c>
       <c r="J108" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K108" s="7">
         <v>0</v>
@@ -9855,7 +9895,7 @@
         <v>187</v>
       </c>
       <c r="F109" s="19" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="G109" s="7" t="s">
         <v>182</v>
@@ -9867,7 +9907,7 @@
         <v>58103</v>
       </c>
       <c r="J109" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K109" s="7">
         <v>0</v>
@@ -9890,7 +9930,7 @@
         <v>3</v>
       </c>
       <c r="F110" s="19" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G110" s="7" t="s">
         <v>182</v>
@@ -9902,7 +9942,7 @@
         <v>58103</v>
       </c>
       <c r="J110" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K110" s="7">
         <v>0</v>
@@ -9925,7 +9965,7 @@
         <v>181</v>
       </c>
       <c r="F111" s="19" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G111" s="7" t="s">
         <v>182</v>
@@ -9934,10 +9974,10 @@
         <v>2</v>
       </c>
       <c r="I111" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="J111" s="19" t="s">
         <v>851</v>
-      </c>
-      <c r="J111" s="19" t="s">
-        <v>852</v>
       </c>
       <c r="K111" s="7">
         <v>0</v>
@@ -9960,7 +10000,7 @@
         <v>0</v>
       </c>
       <c r="F112" s="19" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G112" s="7" t="s">
         <v>182</v>
@@ -9969,10 +10009,10 @@
         <v>2</v>
       </c>
       <c r="I112" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="J112" s="19" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="K112" s="7">
         <v>0</v>
@@ -9995,7 +10035,7 @@
         <v>196</v>
       </c>
       <c r="F113" s="19" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="G113" s="7" t="s">
         <v>182</v>
@@ -10004,10 +10044,10 @@
         <v>2</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="J113" s="19" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="K113" s="7">
         <v>0</v>
@@ -10030,7 +10070,7 @@
         <v>3</v>
       </c>
       <c r="F114" s="19" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="G114" s="7" t="s">
         <v>182</v>
@@ -10039,10 +10079,10 @@
         <v>2</v>
       </c>
       <c r="I114" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="J114" s="19" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="K114" s="7">
         <v>0</v>
@@ -10065,7 +10105,7 @@
         <v>187</v>
       </c>
       <c r="F115" s="19" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G115" s="7" t="s">
         <v>182</v>
@@ -10074,10 +10114,10 @@
         <v>2</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="J115" s="19" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="K115" s="7">
         <v>0</v>
@@ -10100,7 +10140,7 @@
         <v>203</v>
       </c>
       <c r="F116" s="19" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G116" s="7" t="s">
         <v>182</v>
@@ -10109,10 +10149,10 @@
         <v>2</v>
       </c>
       <c r="I116" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="J116" s="19" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="K116" s="7">
         <v>0</v>
@@ -10135,7 +10175,7 @@
         <v>206</v>
       </c>
       <c r="F117" s="19" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G117" s="7" t="s">
         <v>182</v>
@@ -10147,7 +10187,7 @@
         <v>58103</v>
       </c>
       <c r="J117" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K117" s="7">
         <v>0</v>
@@ -10170,7 +10210,7 @@
         <v>209</v>
       </c>
       <c r="F118" s="19" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G118" s="7" t="s">
         <v>182</v>
@@ -10182,7 +10222,7 @@
         <v>58103</v>
       </c>
       <c r="J118" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K118" s="7">
         <v>0</v>
@@ -10205,7 +10245,7 @@
         <v>212</v>
       </c>
       <c r="F119" s="19" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G119" s="7" t="s">
         <v>182</v>
@@ -10217,7 +10257,7 @@
         <v>58103</v>
       </c>
       <c r="J119" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K119" s="7">
         <v>0</v>
@@ -10240,7 +10280,7 @@
         <v>215</v>
       </c>
       <c r="F120" s="19" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G120" s="7" t="s">
         <v>182</v>
@@ -10252,7 +10292,7 @@
         <v>58103</v>
       </c>
       <c r="J120" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K120" s="7">
         <v>0</v>
@@ -10275,7 +10315,7 @@
         <v>218</v>
       </c>
       <c r="F121" s="19" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G121" s="7" t="s">
         <v>182</v>
@@ -10287,7 +10327,7 @@
         <v>58103</v>
       </c>
       <c r="J121" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K121" s="7">
         <v>0</v>
@@ -10310,7 +10350,7 @@
         <v>221</v>
       </c>
       <c r="F122" s="19" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="G122" s="7" t="s">
         <v>182</v>
@@ -10322,7 +10362,7 @@
         <v>58103</v>
       </c>
       <c r="J122" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K122" s="7">
         <v>0</v>
@@ -10339,13 +10379,13 @@
         <v>386</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>387</v>
       </c>
       <c r="F123" s="19" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G123" s="7" t="s">
         <v>116</v>
@@ -10355,7 +10395,7 @@
       </c>
       <c r="I123" s="7"/>
       <c r="J123" s="19" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="K123" s="7">
         <v>0</v>
@@ -10372,13 +10412,13 @@
         <v>222</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>223</v>
       </c>
       <c r="F124" s="19" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="G124" s="7" t="s">
         <v>116</v>
@@ -10390,7 +10430,7 @@
         <v>58109</v>
       </c>
       <c r="J124" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K124" s="7">
         <v>0</v>
@@ -10407,13 +10447,13 @@
         <v>388</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>387</v>
       </c>
       <c r="F125" s="19" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="G125" s="7" t="s">
         <v>116</v>
@@ -10423,7 +10463,7 @@
       </c>
       <c r="I125" s="7"/>
       <c r="J125" s="19" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="K125" s="7">
         <v>0</v>
@@ -10440,13 +10480,13 @@
         <v>224</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>223</v>
       </c>
       <c r="F126" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G126" s="7" t="s">
         <v>116</v>
@@ -10458,7 +10498,7 @@
         <v>58109</v>
       </c>
       <c r="J126" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K126" s="7">
         <v>0</v>
@@ -10475,13 +10515,13 @@
         <v>389</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>390</v>
       </c>
       <c r="F127" s="19" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="G127" s="7" t="s">
         <v>116</v>
@@ -10491,7 +10531,7 @@
       </c>
       <c r="I127" s="7"/>
       <c r="J127" s="19" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="K127" s="7">
         <v>0</v>
@@ -10508,13 +10548,13 @@
         <v>225</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E128" s="7" t="s">
         <v>226</v>
       </c>
       <c r="F128" s="19" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="G128" s="7" t="s">
         <v>116</v>
@@ -10526,7 +10566,7 @@
         <v>58109</v>
       </c>
       <c r="J128" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K128" s="7">
         <v>0</v>
@@ -10543,13 +10583,13 @@
         <v>391</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>390</v>
       </c>
       <c r="F129" s="19" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G129" s="7" t="s">
         <v>116</v>
@@ -10559,7 +10599,7 @@
       </c>
       <c r="I129" s="7"/>
       <c r="J129" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="K129" s="7">
         <v>0</v>
@@ -10576,13 +10616,13 @@
         <v>227</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E130" s="7" t="s">
         <v>226</v>
       </c>
       <c r="F130" s="19" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="G130" s="7" t="s">
         <v>116</v>
@@ -10594,7 +10634,7 @@
         <v>58109</v>
       </c>
       <c r="J130" s="19" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K130" s="7">
         <v>0</v>
@@ -10617,7 +10657,7 @@
         <v>230</v>
       </c>
       <c r="F131" s="19" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="G131" s="7" t="s">
         <v>182</v>
@@ -10629,7 +10669,7 @@
         <v>58116</v>
       </c>
       <c r="J131" s="19" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K131" s="7">
         <v>0</v>
@@ -10652,7 +10692,7 @@
         <v>233</v>
       </c>
       <c r="F132" s="19" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G132" s="7" t="s">
         <v>182</v>
@@ -10664,7 +10704,7 @@
         <v>58116</v>
       </c>
       <c r="J132" s="19" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K132" s="7">
         <v>0</v>
@@ -10687,7 +10727,7 @@
         <v>236</v>
       </c>
       <c r="F133" s="19" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G133" s="7" t="s">
         <v>182</v>
@@ -10699,7 +10739,7 @@
         <v>58117</v>
       </c>
       <c r="J133" s="19" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="K133" s="7">
         <v>0</v>
@@ -10722,7 +10762,7 @@
         <v>239</v>
       </c>
       <c r="F134" s="19" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G134" s="7" t="s">
         <v>182</v>
@@ -10734,7 +10774,7 @@
         <v>58117</v>
       </c>
       <c r="J134" s="19" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="K134" s="7">
         <v>0</v>
@@ -10751,13 +10791,13 @@
         <v>240</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E135" s="7" t="s">
         <v>206</v>
       </c>
       <c r="F135" s="19" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G135" s="7" t="s">
         <v>182</v>
@@ -10769,7 +10809,7 @@
         <v>58119</v>
       </c>
       <c r="J135" s="19" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K135" s="7">
         <v>0</v>
@@ -10786,13 +10826,13 @@
         <v>241</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>209</v>
       </c>
       <c r="F136" s="19" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G136" s="7" t="s">
         <v>182</v>
@@ -10804,7 +10844,7 @@
         <v>58119</v>
       </c>
       <c r="J136" s="19" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="K136" s="7">
         <v>0</v>
@@ -10821,13 +10861,13 @@
         <v>242</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="E137" s="7" t="s">
         <v>209</v>
       </c>
       <c r="F137" s="19" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="G137" s="7" t="s">
         <v>182</v>
@@ -10839,7 +10879,7 @@
         <v>58119</v>
       </c>
       <c r="J137" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="K137" s="7">
         <v>0</v>
@@ -10856,13 +10896,13 @@
         <v>243</v>
       </c>
       <c r="D138" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E138" s="7" t="s">
         <v>215</v>
       </c>
       <c r="F138" s="19" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="G138" s="7" t="s">
         <v>182</v>
@@ -10874,7 +10914,7 @@
         <v>58120</v>
       </c>
       <c r="J138" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="K138" s="7">
         <v>0</v>
@@ -10891,13 +10931,13 @@
         <v>244</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E139" s="7" t="s">
         <v>221</v>
       </c>
       <c r="F139" s="19" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G139" s="7" t="s">
         <v>182</v>
@@ -10909,7 +10949,7 @@
         <v>58120</v>
       </c>
       <c r="J139" s="19" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="K139" s="7">
         <v>0</v>
@@ -10926,13 +10966,13 @@
         <v>245</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>221</v>
       </c>
       <c r="F140" s="19" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G140" s="7" t="s">
         <v>182</v>
@@ -10944,7 +10984,7 @@
         <v>58120</v>
       </c>
       <c r="J140" s="19" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="K140" s="7">
         <v>0</v>
@@ -10961,13 +11001,13 @@
         <v>246</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E141" s="7" t="s">
         <v>230</v>
       </c>
       <c r="F141" s="19" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G141" s="7" t="s">
         <v>182</v>
@@ -10979,7 +11019,7 @@
         <v>58116</v>
       </c>
       <c r="J141" s="19" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="K141" s="7">
         <v>0</v>
@@ -10996,13 +11036,13 @@
         <v>247</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E142" s="7" t="s">
         <v>233</v>
       </c>
       <c r="F142" s="19" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G142" s="7" t="s">
         <v>182</v>
@@ -11014,7 +11054,7 @@
         <v>58116</v>
       </c>
       <c r="J142" s="19" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K142" s="7">
         <v>0</v>
@@ -11031,13 +11071,13 @@
         <v>248</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E143" s="7" t="s">
         <v>236</v>
       </c>
       <c r="F143" s="19" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G143" s="7" t="s">
         <v>182</v>
@@ -11049,7 +11089,7 @@
         <v>58117</v>
       </c>
       <c r="J143" s="19" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K143" s="7">
         <v>0</v>
@@ -11066,13 +11106,13 @@
         <v>249</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E144" s="7" t="s">
         <v>239</v>
       </c>
       <c r="F144" s="19" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G144" s="7" t="s">
         <v>182</v>
@@ -11084,7 +11124,7 @@
         <v>58117</v>
       </c>
       <c r="J144" s="19" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K144" s="7">
         <v>0</v>
@@ -11101,13 +11141,13 @@
         <v>392</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>181</v>
       </c>
       <c r="F145" s="19" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G145" s="7" t="s">
         <v>1</v>
@@ -11117,7 +11157,7 @@
       </c>
       <c r="I145" s="7"/>
       <c r="J145" s="19" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="K145" s="7">
         <v>0</v>
@@ -11134,13 +11174,13 @@
         <v>250</v>
       </c>
       <c r="D146" s="7" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="E146" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F146" s="19" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G146" s="7" t="s">
         <v>1</v>
@@ -11152,7 +11192,7 @@
         <v>58118</v>
       </c>
       <c r="J146" s="19" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="K146" s="7">
         <v>0</v>
@@ -11169,13 +11209,13 @@
         <v>251</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>181</v>
       </c>
       <c r="F147" s="19" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G147" s="7" t="s">
         <v>1</v>
@@ -11187,7 +11227,7 @@
         <v>58118</v>
       </c>
       <c r="J147" s="19" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="K147" s="7">
         <v>0</v>
@@ -11204,13 +11244,13 @@
         <v>393</v>
       </c>
       <c r="D148" s="7" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="E148" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F148" s="19" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="G148" s="7" t="s">
         <v>1</v>
@@ -11220,7 +11260,7 @@
       </c>
       <c r="I148" s="7"/>
       <c r="J148" s="19" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="K148" s="7">
         <v>0</v>
@@ -11237,13 +11277,13 @@
         <v>394</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="E149" s="7" t="s">
         <v>187</v>
       </c>
       <c r="F149" s="19" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="G149" s="7" t="s">
         <v>1</v>
@@ -11253,7 +11293,7 @@
       </c>
       <c r="I149" s="7"/>
       <c r="J149" s="19" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="K149" s="7">
         <v>0</v>
@@ -11270,13 +11310,13 @@
         <v>252</v>
       </c>
       <c r="D150" s="7" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="E150" s="7" t="s">
         <v>3</v>
       </c>
       <c r="F150" s="19" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G150" s="7" t="s">
         <v>1</v>
@@ -11288,7 +11328,7 @@
         <v>58118</v>
       </c>
       <c r="J150" s="19" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="K150" s="7">
         <v>0</v>
@@ -11305,13 +11345,13 @@
         <v>253</v>
       </c>
       <c r="D151" s="7" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="E151" s="7" t="s">
         <v>187</v>
       </c>
       <c r="F151" s="19" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G151" s="7" t="s">
         <v>1</v>
@@ -11323,7 +11363,7 @@
         <v>58118</v>
       </c>
       <c r="J151" s="19" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="K151" s="7">
         <v>0</v>
@@ -11340,13 +11380,13 @@
         <v>395</v>
       </c>
       <c r="D152" s="7" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="E152" s="7" t="s">
         <v>3</v>
       </c>
       <c r="F152" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="G152" s="7" t="s">
         <v>1</v>
@@ -11356,7 +11396,7 @@
       </c>
       <c r="I152" s="7"/>
       <c r="J152" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="K152" s="7">
         <v>0</v>
@@ -11370,22 +11410,22 @@
         <v>140</v>
       </c>
       <c r="C153" s="7" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D153" s="7" t="s">
         <v>1035</v>
       </c>
-      <c r="D153" s="7" t="s">
+      <c r="E153" s="7" t="s">
         <v>1037</v>
       </c>
-      <c r="E153" s="7" t="s">
+      <c r="F153" s="31" t="s">
+        <v>1027</v>
+      </c>
+      <c r="G153" s="7" t="s">
         <v>1039</v>
       </c>
-      <c r="F153" s="31" t="s">
-        <v>1029</v>
-      </c>
-      <c r="G153" s="7" t="s">
-        <v>1041</v>
-      </c>
       <c r="H153" s="9" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I153" s="7">
         <v>58112</v>
@@ -11400,22 +11440,22 @@
         <v>140</v>
       </c>
       <c r="C154" s="7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D154" s="7" t="s">
         <v>1036</v>
       </c>
-      <c r="D154" s="7" t="s">
+      <c r="E154" s="7" t="s">
         <v>1038</v>
       </c>
-      <c r="E154" s="7" t="s">
-        <v>1040</v>
-      </c>
       <c r="F154" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="G154" s="7" t="s">
         <v>80</v>
       </c>
       <c r="H154" s="9" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I154" s="7">
         <v>58112</v>
@@ -20448,7 +20488,7 @@
         <v>605</v>
       </c>
       <c r="C641" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D641" s="18" t="s">
         <v>566</v>
@@ -20462,7 +20502,7 @@
         <v>605</v>
       </c>
       <c r="C642" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D642" s="18" t="s">
         <v>569</v>
@@ -20476,7 +20516,7 @@
         <v>605</v>
       </c>
       <c r="C643" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D643" s="18" t="s">
         <v>570</v>
@@ -20490,7 +20530,7 @@
         <v>605</v>
       </c>
       <c r="C644" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D644" s="18" t="s">
         <v>571</v>
@@ -20504,7 +20544,7 @@
         <v>605</v>
       </c>
       <c r="C645" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D645" s="18" t="s">
         <v>572</v>
@@ -20518,7 +20558,7 @@
         <v>605</v>
       </c>
       <c r="C646" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D646" s="18" t="s">
         <v>573</v>
@@ -20532,7 +20572,7 @@
         <v>605</v>
       </c>
       <c r="C647" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D647" s="18" t="s">
         <v>574</v>
@@ -20546,7 +20586,7 @@
         <v>605</v>
       </c>
       <c r="C648" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D648" s="18" t="s">
         <v>576</v>
@@ -20560,7 +20600,7 @@
         <v>605</v>
       </c>
       <c r="C649" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D649" s="18" t="s">
         <v>577</v>
@@ -20574,7 +20614,7 @@
         <v>605</v>
       </c>
       <c r="C650" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D650" s="18" t="s">
         <v>610</v>
@@ -20588,7 +20628,7 @@
         <v>605</v>
       </c>
       <c r="C651" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D651" s="18" t="s">
         <v>578</v>
@@ -20602,7 +20642,7 @@
         <v>605</v>
       </c>
       <c r="C652" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D652" s="18" t="s">
         <v>580</v>
@@ -20616,7 +20656,7 @@
         <v>605</v>
       </c>
       <c r="C653" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D653" s="18" t="s">
         <v>581</v>
@@ -20630,7 +20670,7 @@
         <v>605</v>
       </c>
       <c r="C654" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D654" s="18" t="s">
         <v>565</v>
@@ -20644,7 +20684,7 @@
         <v>605</v>
       </c>
       <c r="C655" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D655" s="18" t="s">
         <v>569</v>
@@ -20658,7 +20698,7 @@
         <v>605</v>
       </c>
       <c r="C656" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D656" s="18" t="s">
         <v>570</v>
@@ -20672,7 +20712,7 @@
         <v>605</v>
       </c>
       <c r="C657" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D657" s="18" t="s">
         <v>571</v>
@@ -20686,7 +20726,7 @@
         <v>605</v>
       </c>
       <c r="C658" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D658" s="18" t="s">
         <v>572</v>
@@ -20700,7 +20740,7 @@
         <v>605</v>
       </c>
       <c r="C659" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D659" s="18" t="s">
         <v>573</v>
@@ -20714,7 +20754,7 @@
         <v>605</v>
       </c>
       <c r="C660" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D660" s="18" t="s">
         <v>574</v>
@@ -20728,7 +20768,7 @@
         <v>605</v>
       </c>
       <c r="C661" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D661" s="18" t="s">
         <v>606</v>
@@ -20742,7 +20782,7 @@
         <v>605</v>
       </c>
       <c r="C662" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D662" s="18" t="s">
         <v>607</v>
@@ -20756,7 +20796,7 @@
         <v>605</v>
       </c>
       <c r="C663" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D663" s="18" t="s">
         <v>610</v>
@@ -20770,7 +20810,7 @@
         <v>605</v>
       </c>
       <c r="C664" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D664" s="18" t="s">
         <v>578</v>
@@ -20784,7 +20824,7 @@
         <v>605</v>
       </c>
       <c r="C665" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D665" s="18" t="s">
         <v>580</v>
@@ -20798,7 +20838,7 @@
         <v>605</v>
       </c>
       <c r="C666" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D666" s="18" t="s">
         <v>581</v>
@@ -20812,7 +20852,7 @@
         <v>605</v>
       </c>
       <c r="C667" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D667" s="18" t="s">
         <v>567</v>
@@ -20826,7 +20866,7 @@
         <v>605</v>
       </c>
       <c r="C668" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D668" s="18" t="s">
         <v>569</v>
@@ -20840,7 +20880,7 @@
         <v>605</v>
       </c>
       <c r="C669" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D669" s="18" t="s">
         <v>570</v>
@@ -20854,7 +20894,7 @@
         <v>605</v>
       </c>
       <c r="C670" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D670" s="18" t="s">
         <v>571</v>
@@ -20868,7 +20908,7 @@
         <v>605</v>
       </c>
       <c r="C671" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D671" s="18" t="s">
         <v>572</v>
@@ -20882,7 +20922,7 @@
         <v>605</v>
       </c>
       <c r="C672" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D672" s="18" t="s">
         <v>608</v>
@@ -20896,7 +20936,7 @@
         <v>605</v>
       </c>
       <c r="C673" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D673" s="18" t="s">
         <v>575</v>
@@ -20910,7 +20950,7 @@
         <v>605</v>
       </c>
       <c r="C674" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D674" s="18" t="s">
         <v>610</v>
@@ -20924,7 +20964,7 @@
         <v>605</v>
       </c>
       <c r="C675" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D675" s="18" t="s">
         <v>578</v>
@@ -20938,7 +20978,7 @@
         <v>605</v>
       </c>
       <c r="C676" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D676" s="18" t="s">
         <v>580</v>
@@ -20952,7 +20992,7 @@
         <v>605</v>
       </c>
       <c r="C677" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D677" s="18" t="s">
         <v>581</v>
@@ -20963,13 +21003,13 @@
     </row>
     <row r="678" spans="2:5">
       <c r="B678" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C678" s="32" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D678" s="7" t="s">
         <v>1033</v>
-      </c>
-      <c r="D678" s="7" t="s">
-        <v>1035</v>
       </c>
       <c r="E678" s="16">
         <v>0</v>
@@ -20977,13 +21017,13 @@
     </row>
     <row r="679" spans="2:5">
       <c r="B679" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C679" s="32" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D679" s="7" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="E679" s="16">
         <v>0</v>
@@ -20991,13 +21031,13 @@
     </row>
     <row r="680" spans="2:5">
       <c r="B680" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C680" s="32" t="s">
         <v>1032</v>
       </c>
-      <c r="C680" s="32" t="s">
-        <v>1034</v>
-      </c>
       <c r="D680" s="7" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="E680" s="16">
         <v>0</v>
@@ -21005,13 +21045,13 @@
     </row>
     <row r="681" spans="2:5">
       <c r="B681" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C681" s="32" t="s">
         <v>1032</v>
       </c>
-      <c r="C681" s="32" t="s">
-        <v>1034</v>
-      </c>
       <c r="D681" s="7" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="E681" s="16">
         <v>0</v>
@@ -21026,10 +21066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -21189,13 +21229,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="B11" s="4" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -21206,10 +21246,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1042</v>
+        <v>1048</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -21217,13 +21257,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>1005</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>652</v>
+        <v>1047</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1054</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -21234,10 +21274,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>626</v>
+        <v>1003</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>627</v>
+        <v>652</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -21251,7 +21291,7 @@
         <v>626</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>648</v>
+        <v>627</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -21265,23 +21305,23 @@
         <v>626</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>952</v>
+        <v>648</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>951</v>
       </c>
-      <c r="D17" s="22" t="s">
-        <v>953</v>
-      </c>
-      <c r="E17" s="23">
+      <c r="E17" s="5">
         <v>0</v>
       </c>
     </row>
@@ -21290,10 +21330,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="E18" s="23">
         <v>0</v>
@@ -21304,38 +21344,38 @@
         <v>1</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="E19" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="5" t="s">
-        <v>967</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>950</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>956</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="5" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>965</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>966</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>633</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>954</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -21348,8 +21388,8 @@
       <c r="C22" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>956</v>
+      <c r="D22" s="7" t="s">
+        <v>953</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
@@ -21357,13 +21397,13 @@
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="4" t="s">
-        <v>996</v>
+        <v>1</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>997</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>998</v>
+        <v>633</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>955</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -21371,13 +21411,13 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="4" t="s">
-        <v>1</v>
+        <v>994</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>651</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>636</v>
+        <v>995</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>996</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -21388,10 +21428,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>668</v>
+        <v>651</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>636</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>
@@ -21399,13 +21439,13 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>662</v>
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>668</v>
       </c>
       <c r="E26" s="5">
         <v>0</v>
@@ -21413,13 +21453,13 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>686</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>687</v>
+        <v>29</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>662</v>
       </c>
       <c r="E27" s="5">
         <v>0</v>
@@ -21433,7 +21473,7 @@
         <v>686</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E28" s="5">
         <v>0</v>
@@ -21444,10 +21484,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>654</v>
+        <v>686</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>636</v>
+        <v>688</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
@@ -21458,24 +21498,24 @@
         <v>1</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>942</v>
+        <v>654</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="E30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>645</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>646</v>
       </c>
       <c r="E31" s="5">
         <v>0</v>
@@ -21488,8 +21528,8 @@
       <c r="C32" s="6" t="s">
         <v>645</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>42</v>
+      <c r="D32" s="9" t="s">
+        <v>646</v>
       </c>
       <c r="E32" s="5">
         <v>0</v>
@@ -21502,38 +21542,38 @@
       <c r="C33" s="6" t="s">
         <v>645</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="E33" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="29" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>1000</v>
-      </c>
-      <c r="D34" s="30" t="s">
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="29" t="s">
         <v>999</v>
       </c>
-      <c r="E34" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>624</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>646</v>
-      </c>
-      <c r="E35" s="5">
+      <c r="C35" s="29" t="s">
+        <v>998</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>997</v>
+      </c>
+      <c r="E35" s="29">
         <v>0</v>
       </c>
     </row>
@@ -21544,8 +21584,8 @@
       <c r="C36" s="7" t="s">
         <v>624</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>636</v>
+      <c r="D36" s="9" t="s">
+        <v>646</v>
       </c>
       <c r="E36" s="5">
         <v>0</v>
@@ -21556,10 +21596,10 @@
         <v>643</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>1025</v>
+        <v>624</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>652</v>
+        <v>636</v>
       </c>
       <c r="E37" s="5">
         <v>0</v>
@@ -21570,10 +21610,10 @@
         <v>643</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>629</v>
+        <v>1023</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>668</v>
+        <v>652</v>
       </c>
       <c r="E38" s="5">
         <v>0</v>
@@ -21584,10 +21624,10 @@
         <v>643</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>714</v>
+        <v>629</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>713</v>
+        <v>668</v>
       </c>
       <c r="E39" s="5">
         <v>0</v>
@@ -21598,10 +21638,10 @@
         <v>643</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E40" s="5">
         <v>0</v>
@@ -21612,10 +21652,10 @@
         <v>643</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>965</v>
+        <v>719</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>966</v>
+        <v>712</v>
       </c>
       <c r="E41" s="5">
         <v>0</v>
@@ -21625,11 +21665,11 @@
       <c r="B42" s="5" t="s">
         <v>643</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>662</v>
+      <c r="C42" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>965</v>
       </c>
       <c r="E42" s="5">
         <v>0</v>
@@ -21639,11 +21679,11 @@
       <c r="B43" s="5" t="s">
         <v>643</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>686</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>687</v>
+      <c r="C43" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>662</v>
       </c>
       <c r="E43" s="5">
         <v>0</v>
@@ -21657,7 +21697,7 @@
         <v>686</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E44" s="5">
         <v>0</v>
@@ -21668,10 +21708,10 @@
         <v>643</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>654</v>
+        <v>686</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>636</v>
+        <v>688</v>
       </c>
       <c r="E45" s="5">
         <v>0</v>
@@ -21682,52 +21722,52 @@
         <v>643</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>942</v>
+        <v>654</v>
       </c>
       <c r="D46" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="7" t="s">
-        <v>631</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>961</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>632</v>
-      </c>
       <c r="E47" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="7" t="s">
-        <v>631</v>
+      <c r="B48" s="5" t="s">
+        <v>1044</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>962</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>632</v>
+        <v>1043</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>1045</v>
       </c>
       <c r="E48" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:5">
-      <c r="B49" s="7" t="s">
-        <v>631</v>
+      <c r="B49" s="5" t="s">
+        <v>643</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>963</v>
+        <v>1043</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>632</v>
+        <v>1046</v>
       </c>
       <c r="E49" s="5">
         <v>0</v>
@@ -21738,10 +21778,10 @@
         <v>631</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>650</v>
+        <v>632</v>
       </c>
       <c r="E50" s="5">
         <v>0</v>
@@ -21752,10 +21792,10 @@
         <v>631</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>964</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>653</v>
+        <v>961</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>632</v>
       </c>
       <c r="E51" s="5">
         <v>0</v>
@@ -21766,10 +21806,10 @@
         <v>631</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>964</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>682</v>
+        <v>962</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>632</v>
       </c>
       <c r="E52" s="5">
         <v>0</v>
@@ -21777,13 +21817,13 @@
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="7" t="s">
-        <v>983</v>
+        <v>631</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>984</v>
+        <v>963</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>985</v>
+        <v>650</v>
       </c>
       <c r="E53" s="5">
         <v>0</v>
@@ -21794,10 +21834,10 @@
         <v>631</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>658</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>650</v>
+        <v>963</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>653</v>
       </c>
       <c r="E54" s="5">
         <v>0</v>
@@ -21808,10 +21848,10 @@
         <v>631</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>659</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>660</v>
+        <v>963</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>682</v>
       </c>
       <c r="E55" s="5">
         <v>0</v>
@@ -21819,43 +21859,43 @@
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="E56" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="7" t="s">
         <v>631</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C57" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="E57" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="E56" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="22" t="s">
-        <v>631</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>958</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>959</v>
-      </c>
-      <c r="E57" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" s="22" t="s">
-        <v>983</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>958</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>960</v>
-      </c>
-      <c r="E58" s="23">
+      <c r="D58" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="E58" s="5">
         <v>0</v>
       </c>
     </row>
@@ -21864,52 +21904,52 @@
         <v>631</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>629</v>
+        <v>659</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="E59" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:5">
-      <c r="B60" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>988</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>634</v>
-      </c>
-      <c r="E60" s="5">
+      <c r="B60" s="22" t="s">
+        <v>631</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>958</v>
+      </c>
+      <c r="E60" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:5">
-      <c r="B61" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>708</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>634</v>
-      </c>
-      <c r="E61" s="5">
+      <c r="B61" s="22" t="s">
+        <v>981</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>959</v>
+      </c>
+      <c r="E61" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="7" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>647</v>
+        <v>629</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>634</v>
+        <v>668</v>
       </c>
       <c r="E62" s="5">
         <v>0</v>
@@ -21919,8 +21959,8 @@
       <c r="B63" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>703</v>
+      <c r="C63" s="5" t="s">
+        <v>986</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>634</v>
@@ -21933,8 +21973,8 @@
       <c r="B64" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="C64" s="7" t="s">
-        <v>721</v>
+      <c r="C64" s="5" t="s">
+        <v>707</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>634</v>
@@ -21948,7 +21988,7 @@
         <v>635</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>705</v>
+        <v>647</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>634</v>
@@ -21959,13 +21999,13 @@
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="7" t="s">
-        <v>706</v>
+        <v>635</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>664</v>
+        <v>702</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>707</v>
+        <v>634</v>
       </c>
       <c r="E66" s="5">
         <v>0</v>
@@ -21973,13 +22013,13 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="7" t="s">
-        <v>663</v>
+        <v>635</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>665</v>
+        <v>720</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>707</v>
+        <v>634</v>
       </c>
       <c r="E67" s="5">
         <v>0</v>
@@ -21987,13 +22027,13 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="7" t="s">
-        <v>706</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>708</v>
+        <v>635</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>704</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>707</v>
+        <v>634</v>
       </c>
       <c r="E68" s="5">
         <v>0</v>
@@ -22001,13 +22041,13 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="7" t="s">
-        <v>663</v>
+        <v>705</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E69" s="5">
         <v>0</v>
@@ -22018,10 +22058,10 @@
         <v>663</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E70" s="5">
         <v>0</v>
@@ -22029,13 +22069,13 @@
     </row>
     <row r="71" spans="2:5">
       <c r="B71" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>703</v>
+        <v>705</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>707</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E71" s="5">
         <v>0</v>
@@ -22046,10 +22086,10 @@
         <v>663</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>704</v>
+        <v>666</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E72" s="5">
         <v>0</v>
@@ -22060,10 +22100,10 @@
         <v>663</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>705</v>
+        <v>667</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E73" s="5">
         <v>0</v>
@@ -22071,13 +22111,13 @@
     </row>
     <row r="74" spans="2:5">
       <c r="B74" s="7" t="s">
-        <v>628</v>
+        <v>663</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>629</v>
+        <v>702</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>630</v>
+        <v>706</v>
       </c>
       <c r="E74" s="5">
         <v>0</v>
@@ -22085,13 +22125,13 @@
     </row>
     <row r="75" spans="2:5">
       <c r="B75" s="7" t="s">
-        <v>628</v>
+        <v>663</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>655</v>
+        <v>703</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>656</v>
+        <v>706</v>
       </c>
       <c r="E75" s="5">
         <v>0</v>
@@ -22099,13 +22139,13 @@
     </row>
     <row r="76" spans="2:5">
       <c r="B76" s="7" t="s">
-        <v>628</v>
+        <v>663</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>655</v>
+        <v>704</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>657</v>
+        <v>706</v>
       </c>
       <c r="E76" s="5">
         <v>0</v>
@@ -22116,10 +22156,10 @@
         <v>628</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>709</v>
+        <v>629</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>656</v>
+        <v>630</v>
       </c>
       <c r="E77" s="5">
         <v>0</v>
@@ -22130,7 +22170,7 @@
         <v>628</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>710</v>
+        <v>655</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>656</v>
@@ -22141,13 +22181,13 @@
     </row>
     <row r="79" spans="2:5">
       <c r="B79" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>644</v>
+        <v>628</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>655</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>639</v>
+        <v>657</v>
       </c>
       <c r="E79" s="5">
         <v>0</v>
@@ -22155,13 +22195,13 @@
     </row>
     <row r="80" spans="2:5">
       <c r="B80" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>644</v>
+        <v>628</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>708</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>683</v>
+        <v>656</v>
       </c>
       <c r="E80" s="5">
         <v>0</v>
@@ -22169,13 +22209,13 @@
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>640</v>
+        <v>628</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>709</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>641</v>
+        <v>656</v>
       </c>
       <c r="E81" s="5">
         <v>0</v>
@@ -22186,10 +22226,10 @@
         <v>638</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E82" s="5">
         <v>0</v>
@@ -22200,10 +22240,10 @@
         <v>638</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>1006</v>
+        <v>644</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>1007</v>
+        <v>683</v>
       </c>
       <c r="E83" s="5">
         <v>0</v>
@@ -22213,11 +22253,11 @@
       <c r="B84" s="7" t="s">
         <v>638</v>
       </c>
-      <c r="C84" s="6" t="s">
-        <v>1021</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>649</v>
+      <c r="C84" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>641</v>
       </c>
       <c r="E84" s="5">
         <v>0</v>
@@ -22225,13 +22265,13 @@
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="7" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>1023</v>
+        <v>638</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>640</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>1024</v>
+        <v>642</v>
       </c>
       <c r="E85" s="5">
         <v>0</v>
@@ -22239,13 +22279,13 @@
     </row>
     <row r="86" spans="2:5">
       <c r="B86" s="7" t="s">
-        <v>679</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>677</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>680</v>
+        <v>638</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>1005</v>
       </c>
       <c r="E86" s="5">
         <v>0</v>
@@ -22253,13 +22293,13 @@
     </row>
     <row r="87" spans="2:5">
       <c r="B87" s="7" t="s">
-        <v>676</v>
+        <v>638</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>678</v>
+        <v>1019</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>680</v>
+        <v>649</v>
       </c>
       <c r="E87" s="5">
         <v>0</v>
@@ -22267,13 +22307,13 @@
     </row>
     <row r="88" spans="2:5">
       <c r="B88" s="7" t="s">
-        <v>993</v>
+        <v>1020</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>994</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>995</v>
+        <v>1021</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>1022</v>
       </c>
       <c r="E88" s="5">
         <v>0</v>
@@ -22281,13 +22321,13 @@
     </row>
     <row r="89" spans="2:5">
       <c r="B89" s="7" t="s">
-        <v>695</v>
+        <v>679</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>696</v>
+        <v>680</v>
       </c>
       <c r="E89" s="5">
         <v>0</v>
@@ -22295,13 +22335,13 @@
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="7" t="s">
-        <v>685</v>
+        <v>676</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>689</v>
+        <v>680</v>
       </c>
       <c r="E90" s="5">
         <v>0</v>
@@ -22309,13 +22349,13 @@
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="7" t="s">
-        <v>941</v>
+        <v>991</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>686</v>
+        <v>992</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>687</v>
+        <v>993</v>
       </c>
       <c r="E91" s="5">
         <v>0</v>
@@ -22323,13 +22363,13 @@
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="7" t="s">
-        <v>693</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>690</v>
+        <v>694</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>684</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>681</v>
+        <v>695</v>
       </c>
       <c r="E92" s="5">
         <v>0</v>
@@ -22337,13 +22377,13 @@
     </row>
     <row r="93" spans="2:5">
       <c r="B93" s="7" t="s">
-        <v>691</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>690</v>
+        <v>685</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>686</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="E93" s="5">
         <v>0</v>
@@ -22351,13 +22391,13 @@
     </row>
     <row r="94" spans="2:5">
       <c r="B94" s="7" t="s">
-        <v>692</v>
+        <v>940</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>697</v>
+        <v>686</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>698</v>
+        <v>687</v>
       </c>
       <c r="E94" s="5">
         <v>0</v>
@@ -22365,13 +22405,13 @@
     </row>
     <row r="95" spans="2:5">
       <c r="B95" s="7" t="s">
-        <v>700</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>699</v>
+        <v>692</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>690</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>701</v>
+        <v>681</v>
       </c>
       <c r="E95" s="5">
         <v>0</v>
@@ -22379,13 +22419,13 @@
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="7" t="s">
-        <v>700</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>702</v>
+        <v>1051</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>1050</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>701</v>
+        <v>1052</v>
       </c>
       <c r="E96" s="5">
         <v>0</v>
@@ -22393,13 +22433,13 @@
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="7" t="s">
-        <v>700</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>711</v>
+        <v>1053</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>690</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>712</v>
+        <v>693</v>
       </c>
       <c r="E97" s="5">
         <v>0</v>
@@ -22407,13 +22447,13 @@
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="7" t="s">
-        <v>715</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>719</v>
+        <v>1053</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>1050</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>716</v>
+        <v>681</v>
       </c>
       <c r="E98" s="5">
         <v>0</v>
@@ -22421,13 +22461,13 @@
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="7" t="s">
-        <v>715</v>
+        <v>691</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>717</v>
+        <v>696</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>716</v>
+        <v>697</v>
       </c>
       <c r="E99" s="5">
         <v>0</v>
@@ -22435,13 +22475,13 @@
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="7" t="s">
-        <v>715</v>
+        <v>699</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>718</v>
+        <v>698</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>716</v>
+        <v>700</v>
       </c>
       <c r="E100" s="5">
         <v>0</v>
@@ -22449,13 +22489,13 @@
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="7" t="s">
-        <v>986</v>
+        <v>699</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>987</v>
+        <v>701</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>990</v>
+        <v>700</v>
       </c>
       <c r="E101" s="5">
         <v>0</v>
@@ -22463,13 +22503,13 @@
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="7" t="s">
-        <v>986</v>
+        <v>699</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>989</v>
+        <v>710</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>990</v>
+        <v>711</v>
       </c>
       <c r="E102" s="5">
         <v>0</v>
@@ -22477,13 +22517,13 @@
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="7" t="s">
-        <v>986</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>991</v>
+        <v>714</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>718</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>990</v>
+        <v>715</v>
       </c>
       <c r="E103" s="5">
         <v>0</v>
@@ -22491,20 +22531,90 @@
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="7" t="s">
-        <v>986</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>992</v>
+        <v>714</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>716</v>
       </c>
       <c r="D104" s="9" t="s">
+        <v>715</v>
+      </c>
+      <c r="E104" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5">
+      <c r="B105" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>715</v>
+      </c>
+      <c r="E105" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5">
+      <c r="B106" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>985</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>988</v>
+      </c>
+      <c r="E106" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5">
+      <c r="B107" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>987</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>988</v>
+      </c>
+      <c r="E107" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5">
+      <c r="B108" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>988</v>
+      </c>
+      <c r="E108" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5">
+      <c r="B109" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="C109" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="E104" s="5">
+      <c r="D109" s="9" t="s">
+        <v>988</v>
+      </c>
+      <c r="E109" s="5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E101"/>
+  <autoFilter ref="B3:E106"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22585,10 +22695,10 @@
         <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>945</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>946</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>51</v>
@@ -22596,7 +22706,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="20" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>27</v>
@@ -22616,10 +22726,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="20" t="s">
+        <v>942</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>943</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>944</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>28</v>
@@ -22818,7 +22928,7 @@
     </row>
     <row r="4" spans="1:16" ht="27">
       <c r="B4" s="20" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>27</v>
@@ -22845,14 +22955,14 @@
         <v>25</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>949</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>950</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="20" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="O4" s="7">
         <v>58108</v>
@@ -23022,7 +23132,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="24" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>54</v>
@@ -23039,53 +23149,53 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="25" t="s">
+        <v>971</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>973</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>974</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>975</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>976</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="26" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="26" t="s">
+        <v>978</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>967</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>968</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>979</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>980</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>969</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>970</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>981</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>